<commit_message>
Signed-off-by: Manu John <manu.john@cgi.com>
</commit_message>
<xml_diff>
--- a/TestData/TireSearchAdvanced.xlsx
+++ b/TestData/TireSearchAdvanced.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
   <si>
     <t>Run</t>
   </si>
@@ -34,9 +34,15 @@
     <t>Season</t>
   </si>
   <si>
+    <t>BF Goodrich</t>
+  </si>
+  <si>
     <t>All-Season</t>
   </si>
   <si>
+    <t>T</t>
+  </si>
+  <si>
     <t>SpeedRating</t>
   </si>
   <si>
@@ -46,6 +52,12 @@
     <t>AspectRatio</t>
   </si>
   <si>
+    <t>235</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
     <t>275</t>
   </si>
   <si>
@@ -64,28 +76,31 @@
     <t>PC</t>
   </si>
   <si>
+    <t>CT</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>LoadRange</t>
+  </si>
+  <si>
     <t>Remarks</t>
   </si>
   <si>
-    <t>Passenger car - advance search</t>
-  </si>
-  <si>
-    <t>Scenario Type</t>
-  </si>
-  <si>
-    <t>Positive</t>
+    <t>Passenger car - Positive search</t>
+  </si>
+  <si>
+    <t>Commercial Truck - Positive Search</t>
   </si>
   <si>
     <t>Michelin</t>
   </si>
   <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>235</t>
-  </si>
-  <si>
-    <t>19</t>
+    <t>Drive</t>
+  </si>
+  <si>
+    <t>G</t>
   </si>
 </sst>
 </file>
@@ -431,16 +446,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" customWidth="1"/>
-    <col min="2" max="2" width="7.85546875" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
@@ -449,22 +464,22 @@
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.85546875" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" customWidth="1"/>
+    <col min="14" max="14" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -476,30 +491,33 @@
         <v>4</v>
       </c>
       <c r="H1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J1" t="s">
         <v>5</v>
       </c>
       <c r="K1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="M1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C2">
         <v>1002750</v>
@@ -508,39 +526,36 @@
         <v>1276063</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="H2" s="3">
         <v>55</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="M2" t="s">
+      <c r="B3" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
       </c>
       <c r="C3">
         <v>1002750</v>
@@ -549,7 +564,7 @@
         <v>1276063</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2">
         <v>3</v>
@@ -557,36 +572,76 @@
       <c r="H3" s="3"/>
       <c r="I3" s="1"/>
       <c r="J3" t="s">
-        <v>6</v>
-      </c>
-      <c r="L3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="N3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E4" s="1"/>
       <c r="F4" s="2"/>
       <c r="I4" s="1"/>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E5" s="1"/>
-      <c r="F5" s="2"/>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5">
+        <v>1002750</v>
+      </c>
+      <c r="D5">
+        <v>1276063</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
       <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" t="s">
+        <v>28</v>
+      </c>
+      <c r="N5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6">
+        <v>1002750</v>
+      </c>
+      <c r="D6">
+        <v>1276063</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="2"/>
       <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E7" s="1"/>
       <c r="F7" s="2"/>
       <c r="I7" s="1"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E8" s="1"/>
     </row>
   </sheetData>

</xml_diff>